<commit_message>
clear cache and regression
</commit_message>
<xml_diff>
--- a/torgi/output_archive.xlsx
+++ b/torgi/output_archive.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3102" uniqueCount="1680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3104" uniqueCount="1682">
   <si>
     <t>Регион</t>
   </si>
@@ -5057,6 +5057,12 @@
   </si>
   <si>
     <t>52:18:0060027:626</t>
+  </si>
+  <si>
+    <t>Жителей h3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H3 чел/кв.м </t>
   </si>
 </sst>
 </file>
@@ -5108,7 +5114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -5131,6 +5137,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -5139,7 +5156,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5154,12 +5171,45 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -5463,7 +5513,7 @@
   <dimension ref="A1:S441"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5531,6 +5581,12 @@
       <c r="Q1" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="R1" s="9" t="s">
+        <v>1680</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>1681</v>
+      </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="4">
@@ -29644,7 +29700,12 @@
   </sheetData>
   <autoFilter ref="A1:B97"/>
   <conditionalFormatting sqref="L1:L996">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="PP">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="PP">
+      <formula>NOT(ISERROR(SEARCH("PP",L1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="PP">
       <formula>NOT(ISERROR(SEARCH("PP",L1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>